<commit_message>
Homelessness data formatted as csv
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/homeless_figures_parsed.xlsx
+++ b/docs/housing_story_content/homeless_figures_parsed.xlsx
@@ -27,25 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>IN HOTELS</t>
-  </si>
-  <si>
-    <t>IN HOMELESS ACCOMMODATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FAMILIES</t>
-  </si>
-  <si>
-    <t>DEPENDENTS</t>
-  </si>
-  <si>
-    <t>Number of adults with dependent children who are homeless in Dublin</t>
-  </si>
-  <si>
-    <t>June 2015 – July 2016</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>date</t>
   </si>
@@ -370,665 +352,619 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>41791</v>
+      </c>
+      <c r="B2">
+        <v>567</v>
+      </c>
+      <c r="C2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>42552</v>
+        <v>41821</v>
       </c>
       <c r="B3">
-        <v>731</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1490</v>
-      </c>
-      <c r="D3">
-        <v>262</v>
-      </c>
-      <c r="E3">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>595</v>
+      </c>
+      <c r="C3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>41852</v>
+      </c>
+      <c r="B4">
+        <v>640</v>
+      </c>
+      <c r="C4">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B5">
+        <v>668</v>
+      </c>
+      <c r="C5">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B6">
+        <v>680</v>
+      </c>
+      <c r="C6">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>41944</v>
+      </c>
+      <c r="B7">
+        <v>741</v>
+      </c>
+      <c r="C7">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>41791</v>
+        <v>41974</v>
       </c>
       <c r="B8">
-        <v>567</v>
+        <v>726</v>
       </c>
       <c r="C8">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>41821</v>
+        <v>42005</v>
       </c>
       <c r="B9">
-        <v>595</v>
+        <v>780</v>
       </c>
       <c r="C9">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>41852</v>
+        <v>42036</v>
       </c>
       <c r="B10">
-        <v>640</v>
+        <v>803</v>
       </c>
       <c r="C10">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>41883</v>
+        <v>42064</v>
       </c>
       <c r="B11">
-        <v>668</v>
+        <v>911</v>
       </c>
       <c r="C11">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>41913</v>
+        <v>42095</v>
       </c>
       <c r="B12">
-        <v>680</v>
+        <v>970</v>
       </c>
       <c r="C12">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>41944</v>
-      </c>
-      <c r="B13">
-        <v>741</v>
+        <v>42125</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1034</v>
       </c>
       <c r="C13">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>41974</v>
-      </c>
-      <c r="B14">
-        <v>726</v>
+        <v>42156</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1122</v>
       </c>
       <c r="C14">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>42005</v>
-      </c>
-      <c r="B15">
-        <v>780</v>
+        <v>42186</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1185</v>
       </c>
       <c r="C15">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>42036</v>
-      </c>
-      <c r="B16">
-        <v>803</v>
+        <v>42217</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1275</v>
       </c>
       <c r="C16">
-        <v>507</v>
+        <v>832</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>42064</v>
-      </c>
-      <c r="B17">
-        <v>911</v>
+        <v>42248</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1343</v>
       </c>
       <c r="C17">
-        <v>571</v>
+        <v>855</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>42095</v>
-      </c>
-      <c r="B18">
-        <v>970</v>
+        <v>42278</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1425</v>
       </c>
       <c r="C18">
-        <v>616</v>
+        <v>916</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>42125</v>
+        <v>42309</v>
       </c>
       <c r="B19" s="2">
-        <v>1034</v>
+        <v>1466</v>
       </c>
       <c r="C19">
-        <v>677</v>
+        <v>963</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>42156</v>
+        <v>42339</v>
       </c>
       <c r="B20" s="2">
-        <v>1122</v>
+        <v>1409</v>
       </c>
       <c r="C20">
-        <v>729</v>
+        <v>939</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>42186</v>
+        <v>42370</v>
       </c>
       <c r="B21" s="2">
-        <v>1185</v>
-      </c>
-      <c r="C21">
-        <v>770</v>
+        <v>1570</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1042</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>42217</v>
+        <v>42401</v>
       </c>
       <c r="B22" s="2">
-        <v>1275</v>
+        <v>1616</v>
       </c>
       <c r="C22">
-        <v>832</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>42248</v>
+        <v>42430</v>
       </c>
       <c r="B23" s="2">
-        <v>1343</v>
-      </c>
-      <c r="C23">
-        <v>855</v>
+        <v>1723</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1132</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>42278</v>
+        <v>42461</v>
       </c>
       <c r="B24" s="2">
-        <v>1425</v>
-      </c>
-      <c r="C24">
-        <v>916</v>
+        <v>1786</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1188</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>42309</v>
+        <v>42491</v>
       </c>
       <c r="B25" s="2">
-        <v>1466</v>
-      </c>
-      <c r="C25">
-        <v>963</v>
+        <v>1847</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1218</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>42339</v>
+        <v>42522</v>
       </c>
       <c r="B26" s="2">
-        <v>1409</v>
-      </c>
-      <c r="C26">
-        <v>939</v>
+        <v>1894</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1270</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>42370</v>
+        <v>42552</v>
       </c>
       <c r="B27" s="2">
-        <v>1570</v>
+        <v>2020</v>
       </c>
       <c r="C27" s="2">
-        <v>1042</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>42401</v>
+        <v>42583</v>
       </c>
       <c r="B28" s="2">
-        <v>1616</v>
-      </c>
-      <c r="C28">
-        <v>1063</v>
+        <v>2012</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1338</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>42430</v>
+        <v>42614</v>
       </c>
       <c r="B29" s="2">
-        <v>1723</v>
+        <v>2065</v>
       </c>
       <c r="C29" s="2">
-        <v>1132</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>42461</v>
+        <v>42644</v>
       </c>
       <c r="B30" s="2">
-        <v>1786</v>
+        <v>2110</v>
       </c>
       <c r="C30" s="2">
-        <v>1188</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>42491</v>
+        <v>42675</v>
       </c>
       <c r="B31" s="2">
-        <v>1847</v>
+        <v>2110</v>
       </c>
       <c r="C31" s="2">
-        <v>1218</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>42522</v>
+        <v>42705</v>
       </c>
       <c r="B32" s="2">
-        <v>1894</v>
+        <v>2046</v>
       </c>
       <c r="C32" s="2">
-        <v>1270</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>42552</v>
+        <v>42736</v>
       </c>
       <c r="B33" s="2">
-        <v>2020</v>
+        <v>2096</v>
       </c>
       <c r="C33" s="2">
-        <v>1331</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>42583</v>
+        <v>42767</v>
       </c>
       <c r="B34" s="2">
-        <v>2012</v>
+        <v>2129</v>
       </c>
       <c r="C34" s="2">
-        <v>1338</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>42614</v>
+        <v>42795</v>
       </c>
       <c r="B35" s="2">
-        <v>2065</v>
+        <v>2214</v>
       </c>
       <c r="C35" s="2">
-        <v>1357</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>42644</v>
+        <v>42826</v>
       </c>
       <c r="B36" s="2">
-        <v>2110</v>
+        <v>2262</v>
       </c>
       <c r="C36" s="2">
-        <v>1376</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>42675</v>
+        <v>42856</v>
       </c>
       <c r="B37" s="2">
-        <v>2110</v>
+        <v>2266</v>
       </c>
       <c r="C37" s="2">
-        <v>1368</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>42705</v>
+        <v>42887</v>
       </c>
       <c r="B38" s="2">
-        <v>2046</v>
+        <v>2270</v>
       </c>
       <c r="C38" s="2">
-        <v>1353</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>42736</v>
+        <v>42917</v>
       </c>
       <c r="B39" s="2">
-        <v>2096</v>
+        <v>2423</v>
       </c>
       <c r="C39" s="2">
-        <v>1382</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>42767</v>
+        <v>42948</v>
       </c>
       <c r="B40" s="2">
-        <v>2129</v>
+        <v>2379</v>
       </c>
       <c r="C40" s="2">
-        <v>1410</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>42795</v>
+        <v>42979</v>
       </c>
       <c r="B41" s="2">
-        <v>2214</v>
+        <v>2416</v>
       </c>
       <c r="C41" s="2">
-        <v>1426</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>42826</v>
+        <v>43009</v>
       </c>
       <c r="B42" s="2">
-        <v>2262</v>
+        <v>2425</v>
       </c>
       <c r="C42" s="2">
-        <v>1465</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>42856</v>
+        <v>43040</v>
       </c>
       <c r="B43" s="2">
-        <v>2266</v>
+        <v>2533</v>
       </c>
       <c r="C43" s="2">
-        <v>1477</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>42887</v>
+        <v>43070</v>
       </c>
       <c r="B44" s="2">
-        <v>2270</v>
+        <v>2385</v>
       </c>
       <c r="C44" s="2">
-        <v>1492</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>42917</v>
+        <v>43101</v>
       </c>
       <c r="B45" s="2">
-        <v>2423</v>
+        <v>2509</v>
       </c>
       <c r="C45" s="2">
-        <v>1586</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>42948</v>
+        <v>43132</v>
       </c>
       <c r="B46" s="2">
-        <v>2379</v>
+        <v>2801</v>
       </c>
       <c r="C46" s="2">
-        <v>1559</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>42979</v>
+        <v>43160</v>
       </c>
       <c r="B47" s="2">
-        <v>2416</v>
+        <v>2780</v>
       </c>
       <c r="C47" s="2">
-        <v>1562</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43009</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2425</v>
+        <v>43191</v>
+      </c>
+      <c r="B48">
+        <v>2810</v>
       </c>
       <c r="C48" s="2">
-        <v>1561</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43040</v>
+        <v>43221</v>
       </c>
       <c r="B49" s="2">
-        <v>2533</v>
+        <v>2886</v>
       </c>
       <c r="C49" s="2">
-        <v>1632</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>43070</v>
+        <v>43252</v>
       </c>
       <c r="B50" s="2">
-        <v>2385</v>
+        <v>2858</v>
       </c>
       <c r="C50" s="2">
-        <v>1562</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>43101</v>
+        <v>43282</v>
       </c>
       <c r="B51" s="2">
-        <v>2509</v>
+        <v>2894</v>
       </c>
       <c r="C51" s="2">
-        <v>1658</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43132</v>
+        <v>43313</v>
       </c>
       <c r="B52" s="2">
-        <v>2801</v>
+        <v>2821</v>
       </c>
       <c r="C52" s="2">
-        <v>1846</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43160</v>
+        <v>43344</v>
       </c>
       <c r="B53" s="2">
-        <v>2780</v>
+        <v>2869</v>
       </c>
       <c r="C53" s="2">
-        <v>1853</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43191</v>
-      </c>
-      <c r="B54">
-        <v>2810</v>
+        <v>43374</v>
+      </c>
+      <c r="B54" s="2">
+        <v>2800</v>
       </c>
       <c r="C54" s="2">
-        <v>1899</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>43221</v>
+        <v>43405</v>
       </c>
       <c r="B55" s="2">
-        <v>2886</v>
+        <v>2816</v>
       </c>
       <c r="C55" s="2">
-        <v>1859</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>43252</v>
-      </c>
-      <c r="B56" s="2">
-        <v>2858</v>
-      </c>
-      <c r="C56" s="2">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>43282</v>
-      </c>
-      <c r="B57" s="2">
-        <v>2894</v>
-      </c>
-      <c r="C57" s="2">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>43313</v>
-      </c>
-      <c r="B58" s="2">
-        <v>2821</v>
-      </c>
-      <c r="C58" s="2">
-        <v>1821</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>43344</v>
-      </c>
-      <c r="B59" s="2">
-        <v>2869</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>43374</v>
-      </c>
-      <c r="B60" s="2">
-        <v>2800</v>
-      </c>
-      <c r="C60" s="2">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>43405</v>
-      </c>
-      <c r="B61" s="2">
-        <v>2816</v>
-      </c>
-      <c r="C61" s="2">
         <v>1819</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tarce for chart fig 2
</commit_message>
<xml_diff>
--- a/docs/housing_story_content/homeless_figures_parsed.xlsx
+++ b/docs/housing_story_content/homeless_figures_parsed.xlsx
@@ -87,6 +87,3150 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indvidual adults</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>41791.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41821.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41852.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41883.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41913.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41944.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42005.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42036.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42064.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42095.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42125.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42156.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42186.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42217.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42248.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42278.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42309.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42339.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42370.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42401.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42430.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42461.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42491.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42522.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42552.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42583.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42614.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42644.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42675.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42705.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42736.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42767.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42795.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42826.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42856.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42887.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42917.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42948.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42979.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43009.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43040.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43070.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43101.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43132.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43160.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43191.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43221.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43252.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43282.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43313.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43344.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43374.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43405.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>567.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>595.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>668.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>680.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>741.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>726.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>780.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>803.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>911.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>970.0</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>1034.0</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0">
+                  <c:v>1122.0</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="#,##0">
+                  <c:v>1185.0</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="#,##0">
+                  <c:v>1275.0</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="#,##0">
+                  <c:v>1343.0</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="#,##0">
+                  <c:v>1425.0</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>1466.0</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="#,##0">
+                  <c:v>1409.0</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>1570.0</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="#,##0">
+                  <c:v>1616.0</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>1723.0</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>1786.0</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>1847.0</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>1894.0</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>2065.0</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="#,##0">
+                  <c:v>2110.0</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>2110.0</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>2046.0</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>2096.0</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>2129.0</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="#,##0">
+                  <c:v>2214.0</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>2262.0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>2266.0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>2270.0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>2423.0</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>2379.0</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>2416.0</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>2425.0</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>2533.0</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>2385.0</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>2509.0</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>2801.0</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>2780.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2810.0</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>2886.0</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>2858.0</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>2894.0</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>2821.0</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>2869.0</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="#,##0">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="#,##0">
+                  <c:v>2816.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dependents</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>41791.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41821.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41852.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41883.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41913.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41944.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42005.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42036.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42064.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42095.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42125.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42156.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42186.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42217.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42248.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42278.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42309.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42339.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42370.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42401.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42430.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42461.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42491.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42522.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42552.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42583.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42614.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42644.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42675.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42705.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42736.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42767.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42795.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42826.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42856.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42887.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42917.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42948.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42979.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43009.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43040.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43070.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43101.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43132.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43160.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43191.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43221.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43252.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43282.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43313.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43344.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43374.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43405.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>346.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>359.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>387.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>421.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>465.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>493.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>507.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>571.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>616.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>677.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>729.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>770.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>832.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>855.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>916.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>963.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>939.0</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>1042.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1063.0</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>1132.0</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>1188.0</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>1218.0</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>1270.0</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>1331.0</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>1338.0</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>1357.0</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="#,##0">
+                  <c:v>1376.0</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>1368.0</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>1353.0</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>1382.0</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>1410.0</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="#,##0">
+                  <c:v>1426.0</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>1465.0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>1477.0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>1492.0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>1586.0</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>1559.0</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>1562.0</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>1561.0</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>1632.0</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>1562.0</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>1658.0</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>1846.0</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>1853.0</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="#,##0">
+                  <c:v>1899.0</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>1859.0</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>1878.0</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>1896.0</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>1821.0</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>1839.0</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="#,##0">
+                  <c:v>1810.0</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="#,##0">
+                  <c:v>1819.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-779118560"/>
+        <c:axId val="-779116784"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="-779118560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-779116784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="-779116784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-779118560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indvidual adults</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>41791.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41821.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41852.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41883.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41913.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41944.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42005.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42036.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42064.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42095.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42125.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42156.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42186.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42217.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42248.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42278.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42309.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42339.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42370.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42401.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42430.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42461.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42491.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42522.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42552.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42583.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42614.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42644.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42675.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42705.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42736.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42767.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42795.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42826.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42856.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42887.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42917.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42948.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42979.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43009.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43040.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43070.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43101.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43132.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43160.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43191.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43221.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43252.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43282.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43313.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43344.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43374.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43405.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>567.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>595.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>668.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>680.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>741.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>726.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>780.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>803.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>911.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>970.0</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>1034.0</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0">
+                  <c:v>1122.0</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="#,##0">
+                  <c:v>1185.0</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="#,##0">
+                  <c:v>1275.0</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="#,##0">
+                  <c:v>1343.0</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="#,##0">
+                  <c:v>1425.0</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>1466.0</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="#,##0">
+                  <c:v>1409.0</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>1570.0</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="#,##0">
+                  <c:v>1616.0</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>1723.0</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>1786.0</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>1847.0</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>1894.0</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>2020.0</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>2012.0</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>2065.0</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="#,##0">
+                  <c:v>2110.0</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>2110.0</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>2046.0</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>2096.0</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>2129.0</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="#,##0">
+                  <c:v>2214.0</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>2262.0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>2266.0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>2270.0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>2423.0</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>2379.0</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>2416.0</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>2425.0</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>2533.0</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>2385.0</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>2509.0</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>2801.0</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>2780.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2810.0</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>2886.0</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>2858.0</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>2894.0</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>2821.0</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>2869.0</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="#,##0">
+                  <c:v>2800.0</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="#,##0">
+                  <c:v>2816.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dependents</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>41791.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41821.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41852.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41883.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41913.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41944.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42005.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42036.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42064.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42095.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42125.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42156.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42186.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42217.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42248.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42278.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42309.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42339.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42370.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42401.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42430.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42461.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42491.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42522.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42552.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42583.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42614.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>42644.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>42675.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>42705.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>42736.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42767.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>42795.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42826.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42856.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42887.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42917.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42948.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>42979.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>43009.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43040.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43070.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43101.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43132.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43160.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>43191.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43221.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>43252.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>43282.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>43313.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43344.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>43374.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>43405.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>346.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>359.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>387.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>421.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>465.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>493.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>507.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>571.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>616.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>677.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>729.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>770.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>832.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>855.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>916.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>963.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>939.0</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>1042.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1063.0</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="#,##0">
+                  <c:v>1132.0</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="#,##0">
+                  <c:v>1188.0</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>1218.0</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="#,##0">
+                  <c:v>1270.0</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="#,##0">
+                  <c:v>1331.0</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="#,##0">
+                  <c:v>1338.0</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="#,##0">
+                  <c:v>1357.0</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="#,##0">
+                  <c:v>1376.0</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="#,##0">
+                  <c:v>1368.0</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="#,##0">
+                  <c:v>1353.0</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="#,##0">
+                  <c:v>1382.0</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="#,##0">
+                  <c:v>1410.0</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="#,##0">
+                  <c:v>1426.0</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="#,##0">
+                  <c:v>1465.0</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="#,##0">
+                  <c:v>1477.0</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="#,##0">
+                  <c:v>1492.0</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="#,##0">
+                  <c:v>1586.0</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="#,##0">
+                  <c:v>1559.0</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="#,##0">
+                  <c:v>1562.0</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="#,##0">
+                  <c:v>1561.0</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="#,##0">
+                  <c:v>1632.0</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="#,##0">
+                  <c:v>1562.0</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="#,##0">
+                  <c:v>1658.0</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="#,##0">
+                  <c:v>1846.0</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="#,##0">
+                  <c:v>1853.0</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="#,##0">
+                  <c:v>1899.0</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="#,##0">
+                  <c:v>1859.0</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="#,##0">
+                  <c:v>1878.0</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="#,##0">
+                  <c:v>1896.0</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="#,##0">
+                  <c:v>1821.0</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="#,##0">
+                  <c:v>1839.0</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="#,##0">
+                  <c:v>1810.0</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="#,##0">
+                  <c:v>1819.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-776938368"/>
+        <c:axId val="-776936592"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="-776938368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-776936592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="-776936592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-776938368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,8 +3498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,5 +4114,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>